<commit_message>
Adding detail names here so that they can be matched with objet names to avoid errors
</commit_message>
<xml_diff>
--- a/models_table.xlsx
+++ b/models_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noble/Dropbox/1_Research/1_Manuscripts/In_Preparation/Ldeli_growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A4E740-59F4-844E-BB28-11FD7749A990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D201C070-9D9E-5F41-B341-0A1B23CF1F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="3880" windowWidth="21040" windowHeight="12520" xr2:uid="{C576F29D-63E6-6445-8816-0FA6FD0EE95D}"/>
+    <workbookView xWindow="6700" yWindow="3880" windowWidth="24180" windowHeight="12520" xr2:uid="{C576F29D-63E6-6445-8816-0FA6FD0EE95D}"/>
   </bookViews>
   <sheets>
     <sheet name="model structure" sheetId="1" r:id="rId1"/>
@@ -36,59 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
   <si>
     <t>Model Name</t>
   </si>
   <si>
-    <t>Model 1</t>
-  </si>
-  <si>
-    <t>Model 2</t>
-  </si>
-  <si>
-    <t>Model 3</t>
-  </si>
-  <si>
-    <t>Model 4</t>
-  </si>
-  <si>
-    <t>Model 5</t>
-  </si>
-  <si>
-    <t>Model 6</t>
-  </si>
-  <si>
-    <t>Model 7</t>
-  </si>
-  <si>
-    <t>Model 8</t>
-  </si>
-  <si>
-    <t>Model 9</t>
-  </si>
-  <si>
-    <t>Model 10</t>
-  </si>
-  <si>
-    <t>Model 11</t>
-  </si>
-  <si>
-    <t>Model 12</t>
-  </si>
-  <si>
-    <t>Model 13</t>
-  </si>
-  <si>
-    <t>Model 14</t>
-  </si>
-  <si>
-    <t>Model 15</t>
-  </si>
-  <si>
-    <t>Model 16</t>
-  </si>
-  <si>
     <t>Intercept</t>
   </si>
   <si>
@@ -116,17 +68,110 @@
     <t>NO PE</t>
   </si>
   <si>
-    <t>Same as 15</t>
-  </si>
-  <si>
-    <t>Same as 16</t>
+    <t>Name Detail</t>
+  </si>
+  <si>
+    <t>Model 1 - intercepts for G, M, PE</t>
+  </si>
+  <si>
+    <t>Model 2 - linear slopes for G, M, PE</t>
+  </si>
+  <si>
+    <t>Model 3 - quadratic slopes for G, M, PE</t>
+  </si>
+  <si>
+    <t>Model 4 - intercept for G, linear slopes for M, PE</t>
+  </si>
+  <si>
+    <t>Model 5 - intercept for M, linear slopes for G, PE</t>
+  </si>
+  <si>
+    <t>Model 6 - intercept for PE, linear slopes for G, M</t>
+  </si>
+  <si>
+    <t>Model 7 - intercept for PE, quadratic slopes for G, M</t>
+  </si>
+  <si>
+    <t>Model 8 - intercept for PE, quadratic slopes for G, no M</t>
+  </si>
+  <si>
+    <t>Model 9 - quadratic for G, PE, no M</t>
+  </si>
+  <si>
+    <t>Model 10 - intercept for G, M, no PE</t>
+  </si>
+  <si>
+    <t>Model 11 - linear slopes for G, M, no PE</t>
+  </si>
+  <si>
+    <t>Model 12 - quadratic slopes for G, M, no PE</t>
+  </si>
+  <si>
+    <t>Model 13 - quadratic slope for M, intercept for G, no PE</t>
+  </si>
+  <si>
+    <t>Model 14 - quadratic slope for G, intercept for M, no PE</t>
+  </si>
+  <si>
+    <t>Model 15 - quadratic slope for G, no M, no PE</t>
+  </si>
+  <si>
+    <t>Model 16 - linear slope for G, no M, no PE</t>
+  </si>
+  <si>
+    <t>mod_1</t>
+  </si>
+  <si>
+    <t>mod_2</t>
+  </si>
+  <si>
+    <t>mod_3</t>
+  </si>
+  <si>
+    <t>mod_4</t>
+  </si>
+  <si>
+    <t>mod_5</t>
+  </si>
+  <si>
+    <t>mod_6</t>
+  </si>
+  <si>
+    <t>mod_7</t>
+  </si>
+  <si>
+    <t>mod_8</t>
+  </si>
+  <si>
+    <t>mod_9</t>
+  </si>
+  <si>
+    <t>mod_10</t>
+  </si>
+  <si>
+    <t>mod_11</t>
+  </si>
+  <si>
+    <t>mod_12</t>
+  </si>
+  <si>
+    <t>mod_13</t>
+  </si>
+  <si>
+    <t>mod_14</t>
+  </si>
+  <si>
+    <t>mod_15</t>
+  </si>
+  <si>
+    <t>mod_16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +200,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9AA83A"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,7 +242,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A7F9A8-6BD4-2545-BCA1-FAEE02C20FD8}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,17 +580,17 @@
     <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -561,430 +612,475 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J5" s="1"/>
+      <c r="K5" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J7" s="1"/>
+      <c r="K7" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J8" s="1"/>
+      <c r="K8" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
+      <c r="K9" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
+      <c r="K10" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
+      <c r="K11" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J13" s="1"/>
+      <c r="K13" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>11</v>
+      <c r="A14" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" t="s">
-        <v>26</v>
+      <c r="K14" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>12</v>
+      <c r="A15" t="s">
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" t="s">
-        <v>27</v>
+      <c r="K15" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J19" s="1"/>
+      <c r="K19" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added fixed effect models
</commit_message>
<xml_diff>
--- a/models_table.xlsx
+++ b/models_table.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noble/Dropbox/1_Research/1_Manuscripts/In_Preparation/Ldeli_growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A801EB-6612-F748-B6C4-F37097FF4B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA010DB-F001-B242-968A-240CB3FBB47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23320" yWindow="2920" windowWidth="24180" windowHeight="12520" xr2:uid="{C576F29D-63E6-6445-8816-0FA6FD0EE95D}"/>
+    <workbookView xWindow="6920" yWindow="3060" windowWidth="24180" windowHeight="12520" activeTab="1" xr2:uid="{C576F29D-63E6-6445-8816-0FA6FD0EE95D}"/>
   </bookViews>
   <sheets>
-    <sheet name="model structure" sheetId="1" r:id="rId1"/>
+    <sheet name="model structure - Intercept" sheetId="1" r:id="rId1"/>
+    <sheet name="model structure - fixed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="52">
   <si>
     <t>Model Name</t>
   </si>
@@ -168,6 +169,30 @@
   </si>
   <si>
     <t>Note that mod_12 has various variant structures that include: 1) heterogeneous variance (het); 2) full model fixed effects with treatment, linear, quadratic slopes and all interactions (fixed1); fixed2; fixed3; fixed4 are all various combinations of fixed effects without interactions</t>
+  </si>
+  <si>
+    <t>Trt</t>
+  </si>
+  <si>
+    <t>Trt*Linear Slope</t>
+  </si>
+  <si>
+    <t>Trt*Quadratic Slope</t>
+  </si>
+  <si>
+    <t>brm_12_het_fixed1</t>
+  </si>
+  <si>
+    <t>brm_12_het_fixed2</t>
+  </si>
+  <si>
+    <t>brm_12_het_fixed3</t>
+  </si>
+  <si>
+    <t>brm_12_het_fixed4</t>
+  </si>
+  <si>
+    <t>* All models have heterogeneous variance</t>
   </si>
 </sst>
 </file>
@@ -562,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A7F9A8-6BD4-2545-BCA1-FAEE02C20FD8}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,4 +1124,141 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7A989B-172D-4F45-812C-69BC00396168}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>